<commit_message>
System test plan for Manager role
</commit_message>
<xml_diff>
--- a/ModuleTestCases.xlsx
+++ b/ModuleTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6DD2CB-0A15-4CCD-A4E0-AA009119EEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63888845-CB9B-4828-B5DE-A040F7916212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6600" yWindow="195" windowWidth="15375" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -4351,7 +4351,7 @@
   <dimension ref="A1:T99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -21001,7 +21001,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E21" sqref="E21"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:H47"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="35.25" customHeight="1"/>

</xml_diff>